<commit_message>
atualiza a planilha com os jogos da 30 rodada são paulo vs vasco fortaleza vs atlético
</commit_message>
<xml_diff>
--- a/planilhas/planilha_brasileirao_2024.xlsx
+++ b/planilhas/planilha_brasileirao_2024.xlsx
@@ -1917,6 +1917,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
@@ -1927,12 +1933,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1965,25 +1965,25 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -5356,16 +5356,16 @@
         <v>11</v>
       </c>
       <c r="D102" s="6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E102" s="6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F102" s="6">
         <v>90</v>
       </c>
       <c r="G102" s="6">
-        <v>2610</v>
+        <v>2700</v>
       </c>
       <c r="H102" s="6">
         <v>0</v>
@@ -5506,16 +5506,16 @@
         <v>14</v>
       </c>
       <c r="D107" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E107" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F107" s="6">
         <v>75</v>
       </c>
       <c r="G107" s="6">
-        <v>1781</v>
+        <v>1874</v>
       </c>
       <c r="H107" s="6">
         <v>1</v>
@@ -5536,16 +5536,16 @@
         <v>14</v>
       </c>
       <c r="D108" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E108" s="6">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F108" s="6">
         <v>87</v>
       </c>
       <c r="G108" s="6">
-        <v>1302</v>
+        <v>1392</v>
       </c>
       <c r="H108" s="6">
         <v>1</v>
@@ -5566,16 +5566,16 @@
         <v>14</v>
       </c>
       <c r="D109" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E109" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F109" s="6">
         <v>86</v>
       </c>
       <c r="G109" s="6">
-        <v>1899</v>
+        <v>1989</v>
       </c>
       <c r="H109" s="6">
         <v>0</v>
@@ -5596,16 +5596,16 @@
         <v>14</v>
       </c>
       <c r="D110" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E110" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F110" s="6">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G110" s="6">
-        <v>1063</v>
+        <v>1153</v>
       </c>
       <c r="H110" s="6">
         <v>1</v>
@@ -5686,19 +5686,19 @@
         <v>26</v>
       </c>
       <c r="D113" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E113" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F113" s="6">
         <v>50</v>
       </c>
       <c r="G113" s="6">
-        <v>748</v>
+        <v>807</v>
       </c>
       <c r="H113" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I113" s="6">
         <v>2</v>
@@ -5746,16 +5746,16 @@
         <v>26</v>
       </c>
       <c r="D115" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E115" s="6">
         <v>17</v>
       </c>
       <c r="F115" s="6">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G115" s="6">
-        <v>1472</v>
+        <v>1494</v>
       </c>
       <c r="H115" s="6">
         <v>2</v>
@@ -5806,16 +5806,16 @@
         <v>26</v>
       </c>
       <c r="D117" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E117" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F117" s="6">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G117" s="6">
-        <v>1626</v>
+        <v>1716</v>
       </c>
       <c r="H117" s="6">
         <v>3</v>
@@ -5866,22 +5866,22 @@
         <v>26</v>
       </c>
       <c r="D119" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E119" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F119" s="6">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G119" s="6">
-        <v>461</v>
+        <v>529</v>
       </c>
       <c r="H119" s="6">
         <v>0</v>
       </c>
       <c r="I119" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J119" s="4"/>
     </row>
@@ -5896,16 +5896,16 @@
         <v>26</v>
       </c>
       <c r="D120" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E120" s="6">
         <v>9</v>
       </c>
       <c r="F120" s="6">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G120" s="6">
-        <v>766</v>
+        <v>785</v>
       </c>
       <c r="H120" s="6">
         <v>0</v>
@@ -5956,16 +5956,16 @@
         <v>26</v>
       </c>
       <c r="D122" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E122" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F122" s="6">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G122" s="6">
-        <v>917</v>
+        <v>1002</v>
       </c>
       <c r="H122" s="6">
         <v>0</v>
@@ -5986,16 +5986,16 @@
         <v>26</v>
       </c>
       <c r="D123" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E123" s="6">
         <v>12</v>
       </c>
       <c r="F123" s="6">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G123" s="6">
-        <v>1172</v>
+        <v>1190</v>
       </c>
       <c r="H123" s="6">
         <v>0</v>
@@ -6076,16 +6076,16 @@
         <v>39</v>
       </c>
       <c r="D126" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E126" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F126" s="6">
         <v>66</v>
       </c>
       <c r="G126" s="6">
-        <v>1523</v>
+        <v>1590</v>
       </c>
       <c r="H126" s="6">
         <v>8</v>
@@ -6106,16 +6106,16 @@
         <v>39</v>
       </c>
       <c r="D127" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E127" s="6">
         <v>21</v>
       </c>
       <c r="F127" s="6">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G127" s="6">
-        <v>1671</v>
+        <v>1694</v>
       </c>
       <c r="H127" s="6">
         <v>4</v>
@@ -6136,16 +6136,16 @@
         <v>39</v>
       </c>
       <c r="D128" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E128" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F128" s="6">
         <v>36</v>
       </c>
       <c r="G128" s="6">
-        <v>611</v>
+        <v>687</v>
       </c>
       <c r="H128" s="6">
         <v>2</v>
@@ -6166,16 +6166,16 @@
         <v>39</v>
       </c>
       <c r="D129" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E129" s="6">
         <v>13</v>
       </c>
       <c r="F129" s="6">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G129" s="6">
-        <v>1158</v>
+        <v>1168</v>
       </c>
       <c r="H129" s="6">
         <v>5</v>
@@ -7096,16 +7096,16 @@
         <v>11</v>
       </c>
       <c r="D160" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E160" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F160" s="6">
         <v>90</v>
       </c>
       <c r="G160" s="6">
-        <v>1530</v>
+        <v>1620</v>
       </c>
       <c r="H160" s="6">
         <v>0</v>
@@ -7306,16 +7306,16 @@
         <v>14</v>
       </c>
       <c r="D167" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E167" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F167" s="6">
         <v>77</v>
       </c>
       <c r="G167" s="6">
-        <v>1611</v>
+        <v>1701</v>
       </c>
       <c r="H167" s="6">
         <v>0</v>
@@ -7336,16 +7336,16 @@
         <v>14</v>
       </c>
       <c r="D168" s="6">
+        <v>22</v>
+      </c>
+      <c r="E168" s="6">
         <v>21</v>
-      </c>
-      <c r="E168" s="6">
-        <v>20</v>
       </c>
       <c r="F168" s="6">
         <v>82</v>
       </c>
       <c r="G168" s="6">
-        <v>1713</v>
+        <v>1803</v>
       </c>
       <c r="H168" s="6">
         <v>0</v>
@@ -7475,7 +7475,7 @@
       </c>
       <c r="J172" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="19.5">
       <c r="A173" s="5" t="s">
         <v>173</v>
       </c>
@@ -7486,16 +7486,16 @@
         <v>14</v>
       </c>
       <c r="D173" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E173" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F173" s="6">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G173" s="6">
-        <v>540</v>
+        <v>623</v>
       </c>
       <c r="H173" s="6">
         <v>0</v>
@@ -7505,7 +7505,7 @@
       </c>
       <c r="J173" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="19.5">
       <c r="A174" s="5" t="s">
         <v>173</v>
       </c>
@@ -7516,16 +7516,16 @@
         <v>14</v>
       </c>
       <c r="D174" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E174" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F174" s="6">
         <v>90</v>
       </c>
       <c r="G174" s="6">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="H174" s="6">
         <v>0</v>
@@ -7535,7 +7535,7 @@
       </c>
       <c r="J174" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="19.5">
       <c r="A175" s="5" t="s">
         <v>173</v>
       </c>
@@ -7565,7 +7565,7 @@
       </c>
       <c r="J175" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="19.5">
       <c r="A176" s="5" t="s">
         <v>173</v>
       </c>
@@ -7576,26 +7576,26 @@
         <v>26</v>
       </c>
       <c r="D176" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E176" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F176" s="6">
         <v>78</v>
       </c>
       <c r="G176" s="6">
-        <v>1553</v>
+        <v>1631</v>
       </c>
       <c r="H176" s="6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I176" s="6">
         <v>4</v>
       </c>
       <c r="J176" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="19.5">
       <c r="A177" s="5" t="s">
         <v>173</v>
       </c>
@@ -7606,26 +7606,26 @@
         <v>26</v>
       </c>
       <c r="D177" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E177" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F177" s="6">
         <v>72</v>
       </c>
       <c r="G177" s="6">
-        <v>1646</v>
+        <v>1723</v>
       </c>
       <c r="H177" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I177" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J177" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="19.5">
       <c r="A178" s="5" t="s">
         <v>173</v>
       </c>
@@ -7655,7 +7655,7 @@
       </c>
       <c r="J178" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="19.5">
       <c r="A179" s="5" t="s">
         <v>173</v>
       </c>
@@ -7666,16 +7666,16 @@
         <v>26</v>
       </c>
       <c r="D179" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E179" s="6">
         <v>3</v>
       </c>
       <c r="F179" s="6">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G179" s="6">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="H179" s="6">
         <v>0</v>
@@ -7685,7 +7685,7 @@
       </c>
       <c r="J179" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="19.5">
       <c r="A180" s="5" t="s">
         <v>173</v>
       </c>
@@ -7696,16 +7696,16 @@
         <v>26</v>
       </c>
       <c r="D180" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E180" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F180" s="6">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G180" s="6">
-        <v>1505</v>
+        <v>1595</v>
       </c>
       <c r="H180" s="6">
         <v>0</v>
@@ -7715,7 +7715,7 @@
       </c>
       <c r="J180" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="19.5">
       <c r="A181" s="5" t="s">
         <v>173</v>
       </c>
@@ -7726,16 +7726,16 @@
         <v>26</v>
       </c>
       <c r="D181" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E181" s="6">
         <v>9</v>
       </c>
       <c r="F181" s="6">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G181" s="6">
-        <v>842</v>
+        <v>855</v>
       </c>
       <c r="H181" s="6">
         <v>0</v>
@@ -7745,7 +7745,7 @@
       </c>
       <c r="J181" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="19.5">
       <c r="A182" s="5" t="s">
         <v>173</v>
       </c>
@@ -7775,7 +7775,7 @@
       </c>
       <c r="J182" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="19.5">
       <c r="A183" s="5" t="s">
         <v>173</v>
       </c>
@@ -7786,26 +7786,26 @@
         <v>26</v>
       </c>
       <c r="D183" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E183" s="6">
         <v>10</v>
       </c>
       <c r="F183" s="6">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G183" s="6">
-        <v>937</v>
+        <v>961</v>
       </c>
       <c r="H183" s="6">
         <v>0</v>
       </c>
       <c r="I183" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J183" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="19.5">
       <c r="A184" s="5" t="s">
         <v>173</v>
       </c>
@@ -7835,7 +7835,7 @@
       </c>
       <c r="J184" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="19.5">
       <c r="A185" s="5" t="s">
         <v>173</v>
       </c>
@@ -7846,16 +7846,16 @@
         <v>26</v>
       </c>
       <c r="D185" s="6">
+        <v>6</v>
+      </c>
+      <c r="E185" s="6">
         <v>5</v>
       </c>
-      <c r="E185" s="6">
-        <v>4</v>
-      </c>
       <c r="F185" s="6">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G185" s="6">
-        <v>369</v>
+        <v>452</v>
       </c>
       <c r="H185" s="6">
         <v>0</v>
@@ -7865,7 +7865,7 @@
       </c>
       <c r="J185" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="19.5">
       <c r="A186" s="5" t="s">
         <v>173</v>
       </c>
@@ -7895,7 +7895,7 @@
       </c>
       <c r="J186" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="19.5">
       <c r="A187" s="5" t="s">
         <v>173</v>
       </c>
@@ -7925,7 +7925,7 @@
       </c>
       <c r="J187" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="19.5">
       <c r="A188" s="5" t="s">
         <v>173</v>
       </c>
@@ -7955,7 +7955,7 @@
       </c>
       <c r="J188" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="19.5">
       <c r="A189" s="5" t="s">
         <v>173</v>
       </c>
@@ -7985,7 +7985,7 @@
       </c>
       <c r="J189" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="19.5">
       <c r="A190" s="5" t="s">
         <v>173</v>
       </c>
@@ -7996,16 +7996,16 @@
         <v>26</v>
       </c>
       <c r="D190" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E190" s="6">
         <v>1</v>
       </c>
       <c r="F190" s="6">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="G190" s="6">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="H190" s="6">
         <v>0</v>
@@ -8015,7 +8015,7 @@
       </c>
       <c r="J190" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="19.5">
       <c r="A191" s="5" t="s">
         <v>173</v>
       </c>
@@ -8045,7 +8045,7 @@
       </c>
       <c r="J191" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="19.5">
       <c r="A192" s="5" t="s">
         <v>173</v>
       </c>
@@ -8056,26 +8056,26 @@
         <v>39</v>
       </c>
       <c r="D192" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E192" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F192" s="6">
         <v>74</v>
       </c>
       <c r="G192" s="6">
-        <v>1697</v>
+        <v>1787</v>
       </c>
       <c r="H192" s="6">
         <v>5</v>
       </c>
       <c r="I192" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J192" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="19.5">
       <c r="A193" s="5" t="s">
         <v>173</v>
       </c>
@@ -8086,16 +8086,16 @@
         <v>39</v>
       </c>
       <c r="D193" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E193" s="6">
         <v>9</v>
       </c>
       <c r="F193" s="6">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G193" s="6">
-        <v>849</v>
+        <v>861</v>
       </c>
       <c r="H193" s="6">
         <v>5</v>
@@ -8105,7 +8105,7 @@
       </c>
       <c r="J193" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="19.5">
       <c r="A194" s="5" t="s">
         <v>173</v>
       </c>
@@ -8135,7 +8135,7 @@
       </c>
       <c r="J194" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="19.5">
       <c r="A195" s="5" t="s">
         <v>173</v>
       </c>
@@ -8146,16 +8146,16 @@
         <v>39</v>
       </c>
       <c r="D195" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E195" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F195" s="6">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G195" s="6">
-        <v>449</v>
+        <v>515</v>
       </c>
       <c r="H195" s="6">
         <v>1</v>
@@ -8165,7 +8165,7 @@
       </c>
       <c r="J195" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="19.5">
       <c r="A196" s="5" t="s">
         <v>173</v>
       </c>
@@ -8195,7 +8195,7 @@
       </c>
       <c r="J196" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="19.5">
       <c r="A197" s="5" t="s">
         <v>173</v>
       </c>
@@ -8225,7 +8225,7 @@
       </c>
       <c r="J197" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="19.5">
       <c r="A198" s="5" t="s">
         <v>211</v>
       </c>
@@ -8255,7 +8255,7 @@
       </c>
       <c r="J198" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="19.5">
       <c r="A199" s="5" t="s">
         <v>211</v>
       </c>
@@ -8285,7 +8285,7 @@
       </c>
       <c r="J199" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="19.5">
       <c r="A200" s="5" t="s">
         <v>211</v>
       </c>
@@ -11026,16 +11026,16 @@
         <v>11</v>
       </c>
       <c r="D291" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E291" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F291" s="6">
         <v>90</v>
       </c>
       <c r="G291" s="6">
-        <v>1523</v>
+        <v>1613</v>
       </c>
       <c r="H291" s="6">
         <v>0</v>
@@ -11176,16 +11176,16 @@
         <v>14</v>
       </c>
       <c r="D296" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E296" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F296" s="6">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G296" s="6">
-        <v>1525</v>
+        <v>1615</v>
       </c>
       <c r="H296" s="6">
         <v>0</v>
@@ -11206,16 +11206,16 @@
         <v>14</v>
       </c>
       <c r="D297" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E297" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F297" s="6">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G297" s="6">
-        <v>1581</v>
+        <v>1671</v>
       </c>
       <c r="H297" s="6">
         <v>0</v>
@@ -11266,16 +11266,16 @@
         <v>14</v>
       </c>
       <c r="D299" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E299" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F299" s="6">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G299" s="6">
-        <v>560</v>
+        <v>650</v>
       </c>
       <c r="H299" s="6">
         <v>0</v>
@@ -11296,16 +11296,16 @@
         <v>14</v>
       </c>
       <c r="D300" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E300" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F300" s="6">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G300" s="6">
-        <v>424</v>
+        <v>514</v>
       </c>
       <c r="H300" s="6">
         <v>0</v>
@@ -11386,16 +11386,16 @@
         <v>26</v>
       </c>
       <c r="D303" s="6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E303" s="6">
         <v>21</v>
       </c>
       <c r="F303" s="6">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G303" s="6">
-        <v>1869</v>
+        <v>1879</v>
       </c>
       <c r="H303" s="6">
         <v>4</v>
@@ -11416,19 +11416,19 @@
         <v>26</v>
       </c>
       <c r="D304" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E304" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F304" s="6">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G304" s="6">
-        <v>1168</v>
+        <v>1258</v>
       </c>
       <c r="H304" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I304" s="6">
         <v>0</v>
@@ -11536,16 +11536,16 @@
         <v>26</v>
       </c>
       <c r="D308" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E308" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F308" s="6">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G308" s="6">
-        <v>1023</v>
+        <v>1103</v>
       </c>
       <c r="H308" s="6">
         <v>1</v>
@@ -11626,16 +11626,16 @@
         <v>26</v>
       </c>
       <c r="D311" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E311" s="6">
         <v>17</v>
       </c>
       <c r="F311" s="6">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G311" s="6">
-        <v>1433</v>
+        <v>1448</v>
       </c>
       <c r="H311" s="6">
         <v>0</v>
@@ -11656,16 +11656,16 @@
         <v>26</v>
       </c>
       <c r="D312" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E312" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F312" s="6">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G312" s="6">
-        <v>484</v>
+        <v>564</v>
       </c>
       <c r="H312" s="6">
         <v>0</v>
@@ -11686,22 +11686,22 @@
         <v>26</v>
       </c>
       <c r="D313" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E313" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F313" s="6">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G313" s="6">
-        <v>637</v>
+        <v>708</v>
       </c>
       <c r="H313" s="6">
         <v>2</v>
       </c>
       <c r="I313" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J313" s="4"/>
     </row>
@@ -11716,16 +11716,16 @@
         <v>26</v>
       </c>
       <c r="D314" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E314" s="6">
         <v>0</v>
       </c>
       <c r="F314" s="6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G314" s="6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H314" s="6">
         <v>0</v>
@@ -11746,16 +11746,16 @@
         <v>26</v>
       </c>
       <c r="D315" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E315" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F315" s="6">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G315" s="6">
-        <v>302</v>
+        <v>391</v>
       </c>
       <c r="H315" s="6">
         <v>0</v>
@@ -11926,16 +11926,16 @@
         <v>39</v>
       </c>
       <c r="D321" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E321" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F321" s="6">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G321" s="6">
-        <v>124</v>
+        <v>214</v>
       </c>
       <c r="H321" s="6">
         <v>0</v>
@@ -11986,16 +11986,16 @@
         <v>11</v>
       </c>
       <c r="D323" s="6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E323" s="6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F323" s="6">
         <v>90</v>
       </c>
       <c r="G323" s="6">
-        <v>2520</v>
+        <v>2610</v>
       </c>
       <c r="H323" s="6">
         <v>0</v>
@@ -12076,16 +12076,16 @@
         <v>14</v>
       </c>
       <c r="D326" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E326" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F326" s="6">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G326" s="6">
-        <v>2020</v>
+        <v>2079</v>
       </c>
       <c r="H326" s="6">
         <v>1</v>
@@ -12106,16 +12106,16 @@
         <v>14</v>
       </c>
       <c r="D327" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E327" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F327" s="6">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G327" s="6">
-        <v>1017</v>
+        <v>1107</v>
       </c>
       <c r="H327" s="6">
         <v>1</v>
@@ -12166,7 +12166,7 @@
         <v>14</v>
       </c>
       <c r="D329" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E329" s="6">
         <v>5</v>
@@ -12175,7 +12175,7 @@
         <v>40</v>
       </c>
       <c r="G329" s="6">
-        <v>517</v>
+        <v>562</v>
       </c>
       <c r="H329" s="6">
         <v>0</v>
@@ -12196,16 +12196,16 @@
         <v>14</v>
       </c>
       <c r="D330" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E330" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F330" s="6">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G330" s="6">
-        <v>1984</v>
+        <v>2074</v>
       </c>
       <c r="H330" s="6">
         <v>1</v>
@@ -12256,16 +12256,16 @@
         <v>14</v>
       </c>
       <c r="D332" s="6">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E332" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F332" s="6">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G332" s="6">
-        <v>1973</v>
+        <v>2018</v>
       </c>
       <c r="H332" s="6">
         <v>1</v>
@@ -12316,16 +12316,16 @@
         <v>26</v>
       </c>
       <c r="D334" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E334" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F334" s="6">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G334" s="6">
-        <v>227</v>
+        <v>303</v>
       </c>
       <c r="H334" s="6">
         <v>1</v>
@@ -12346,16 +12346,16 @@
         <v>26</v>
       </c>
       <c r="D335" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E335" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F335" s="6">
         <v>59</v>
       </c>
       <c r="G335" s="6">
-        <v>830</v>
+        <v>889</v>
       </c>
       <c r="H335" s="6">
         <v>1</v>
@@ -12466,16 +12466,16 @@
         <v>26</v>
       </c>
       <c r="D339" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E339" s="6">
         <v>9</v>
       </c>
       <c r="F339" s="6">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G339" s="6">
-        <v>774</v>
+        <v>788</v>
       </c>
       <c r="H339" s="6">
         <v>0</v>
@@ -12526,16 +12526,16 @@
         <v>26</v>
       </c>
       <c r="D341" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E341" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F341" s="6">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G341" s="6">
-        <v>1463</v>
+        <v>1553</v>
       </c>
       <c r="H341" s="6">
         <v>0</v>
@@ -12586,16 +12586,16 @@
         <v>26</v>
       </c>
       <c r="D343" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E343" s="6">
         <v>1</v>
       </c>
       <c r="F343" s="6">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="G343" s="6">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="H343" s="6">
         <v>0</v>
@@ -12646,16 +12646,16 @@
         <v>26</v>
       </c>
       <c r="D345" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E345" s="6">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F345" s="6">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G345" s="6">
-        <v>1407</v>
+        <v>1497</v>
       </c>
       <c r="H345" s="6">
         <v>2</v>
@@ -12676,16 +12676,16 @@
         <v>26</v>
       </c>
       <c r="D346" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E346" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F346" s="6">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G346" s="6">
-        <v>440</v>
+        <v>530</v>
       </c>
       <c r="H346" s="6">
         <v>1</v>
@@ -12826,16 +12826,16 @@
         <v>39</v>
       </c>
       <c r="D351" s="6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E351" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F351" s="6">
         <v>87</v>
       </c>
       <c r="G351" s="6">
-        <v>2264</v>
+        <v>2340</v>
       </c>
       <c r="H351" s="6">
         <v>9</v>
@@ -12856,7 +12856,7 @@
         <v>39</v>
       </c>
       <c r="D352" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E352" s="6">
         <v>5</v>
@@ -12865,7 +12865,7 @@
         <v>34</v>
       </c>
       <c r="G352" s="6">
-        <v>615</v>
+        <v>646</v>
       </c>
       <c r="H352" s="6">
         <v>1</v>

</xml_diff>

<commit_message>
fix: Planilha brasileirão atualizada
</commit_message>
<xml_diff>
--- a/planilhas/planilha_brasileirao_2024.xlsx
+++ b/planilhas/planilha_brasileirao_2024.xlsx
@@ -2356,16 +2356,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="7">
         <v>90</v>
       </c>
       <c r="G2" s="6">
-        <v>1170</v>
+        <v>1260</v>
       </c>
       <c r="H2" s="6">
         <v>0</v>
@@ -2476,19 +2476,19 @@
         <v>14</v>
       </c>
       <c r="D6" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="6">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G6" s="6">
-        <v>1534</v>
+        <v>1624</v>
       </c>
       <c r="H6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="6">
         <v>0</v>
@@ -2536,16 +2536,16 @@
         <v>14</v>
       </c>
       <c r="D8" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8" s="6">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G8" s="6">
-        <v>873</v>
+        <v>963</v>
       </c>
       <c r="H8" s="6">
         <v>0</v>
@@ -2596,16 +2596,16 @@
         <v>14</v>
       </c>
       <c r="D10" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E10" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F10" s="6">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G10" s="6">
-        <v>781</v>
+        <v>871</v>
       </c>
       <c r="H10" s="6">
         <v>1</v>
@@ -2626,19 +2626,19 @@
         <v>14</v>
       </c>
       <c r="D11" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E11" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F11" s="6">
         <v>89</v>
       </c>
       <c r="G11" s="6">
-        <v>2055</v>
+        <v>2145</v>
       </c>
       <c r="H11" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I11" s="6">
         <v>1</v>
@@ -2746,22 +2746,22 @@
         <v>26</v>
       </c>
       <c r="D15" s="6">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E15" s="6">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F15" s="6">
         <v>85</v>
       </c>
       <c r="G15" s="6">
-        <v>2288</v>
+        <v>2373</v>
       </c>
       <c r="H15" s="6">
+        <v>6</v>
+      </c>
+      <c r="I15" s="6">
         <v>5</v>
-      </c>
-      <c r="I15" s="6">
-        <v>4</v>
       </c>
       <c r="J15" s="4"/>
     </row>
@@ -2776,16 +2776,16 @@
         <v>26</v>
       </c>
       <c r="D16" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E16" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="6">
         <v>49</v>
       </c>
       <c r="G16" s="6">
-        <v>160</v>
+        <v>244</v>
       </c>
       <c r="H16" s="6">
         <v>0</v>
@@ -2806,16 +2806,16 @@
         <v>26</v>
       </c>
       <c r="D17" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E17" s="6">
         <v>10</v>
       </c>
       <c r="F17" s="6">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G17" s="6">
-        <v>1210</v>
+        <v>1220</v>
       </c>
       <c r="H17" s="6">
         <v>1</v>
@@ -2836,16 +2836,16 @@
         <v>26</v>
       </c>
       <c r="D18" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E18" s="6">
         <v>21</v>
       </c>
       <c r="F18" s="6">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G18" s="6">
-        <v>1769</v>
+        <v>1780</v>
       </c>
       <c r="H18" s="6">
         <v>0</v>
@@ -2866,16 +2866,16 @@
         <v>26</v>
       </c>
       <c r="D19" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E19" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F19" s="6">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G19" s="6">
-        <v>1238</v>
+        <v>1283</v>
       </c>
       <c r="H19" s="6">
         <v>0</v>
@@ -2896,16 +2896,16 @@
         <v>26</v>
       </c>
       <c r="D20" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E20" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F20" s="6">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G20" s="6">
-        <v>383</v>
+        <v>448</v>
       </c>
       <c r="H20" s="6">
         <v>0</v>
@@ -3016,16 +3016,16 @@
         <v>26</v>
       </c>
       <c r="D24" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E24" s="6">
         <v>5</v>
       </c>
       <c r="F24" s="6">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G24" s="6">
-        <v>467</v>
+        <v>492</v>
       </c>
       <c r="H24" s="6">
         <v>0</v>
@@ -3106,19 +3106,19 @@
         <v>39</v>
       </c>
       <c r="D27" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E27" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="6">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="G27" s="6">
-        <v>138</v>
+        <v>214</v>
       </c>
       <c r="H27" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="6">
         <v>1</v>
@@ -3136,19 +3136,19 @@
         <v>39</v>
       </c>
       <c r="D28" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E28" s="6">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F28" s="6">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G28" s="6">
-        <v>1671</v>
+        <v>1761</v>
       </c>
       <c r="H28" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I28" s="6">
         <v>4</v>
@@ -3166,7 +3166,7 @@
         <v>39</v>
       </c>
       <c r="D29" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E29" s="6">
         <v>15</v>
@@ -3175,7 +3175,7 @@
         <v>63</v>
       </c>
       <c r="G29" s="6">
-        <v>1268</v>
+        <v>1313</v>
       </c>
       <c r="H29" s="6">
         <v>5</v>
@@ -3196,22 +3196,22 @@
         <v>39</v>
       </c>
       <c r="D30" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E30" s="6">
         <v>4</v>
       </c>
       <c r="F30" s="6">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G30" s="6">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="H30" s="6">
         <v>2</v>
       </c>
       <c r="I30" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="4"/>
     </row>
@@ -6226,16 +6226,16 @@
         <v>11</v>
       </c>
       <c r="D131" s="6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E131" s="6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F131" s="6">
         <v>90</v>
       </c>
       <c r="G131" s="6">
-        <v>2340</v>
+        <v>2430</v>
       </c>
       <c r="H131" s="6">
         <v>0</v>
@@ -6316,16 +6316,16 @@
         <v>14</v>
       </c>
       <c r="D134" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E134" s="6">
         <v>1</v>
       </c>
       <c r="F134" s="6">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="G134" s="6">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="H134" s="6">
         <v>0</v>
@@ -6346,16 +6346,16 @@
         <v>14</v>
       </c>
       <c r="D135" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E135" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F135" s="6">
         <v>74</v>
       </c>
       <c r="G135" s="6">
-        <v>1769</v>
+        <v>1840</v>
       </c>
       <c r="H135" s="6">
         <v>2</v>
@@ -6406,16 +6406,16 @@
         <v>14</v>
       </c>
       <c r="D137" s="6">
+        <v>22</v>
+      </c>
+      <c r="E137" s="6">
         <v>21</v>
-      </c>
-      <c r="E137" s="6">
-        <v>20</v>
       </c>
       <c r="F137" s="6">
         <v>84</v>
       </c>
       <c r="G137" s="6">
-        <v>1767</v>
+        <v>1857</v>
       </c>
       <c r="H137" s="6">
         <v>1</v>
@@ -6436,16 +6436,16 @@
         <v>14</v>
       </c>
       <c r="D138" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E138" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F138" s="6">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G138" s="6">
-        <v>1558</v>
+        <v>1648</v>
       </c>
       <c r="H138" s="6">
         <v>0</v>
@@ -6496,16 +6496,16 @@
         <v>14</v>
       </c>
       <c r="D140" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E140" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F140" s="6">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G140" s="6">
-        <v>1704</v>
+        <v>1794</v>
       </c>
       <c r="H140" s="6">
         <v>0</v>
@@ -6526,16 +6526,16 @@
         <v>14</v>
       </c>
       <c r="D141" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E141" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F141" s="6">
         <v>72</v>
       </c>
       <c r="G141" s="6">
-        <v>1370</v>
+        <v>1432</v>
       </c>
       <c r="H141" s="6">
         <v>0</v>
@@ -6586,16 +6586,16 @@
         <v>26</v>
       </c>
       <c r="D143" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E143" s="6">
         <v>10</v>
       </c>
       <c r="F143" s="6">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G143" s="6">
-        <v>899</v>
+        <v>918</v>
       </c>
       <c r="H143" s="6">
         <v>4</v>
@@ -6616,16 +6616,16 @@
         <v>26</v>
       </c>
       <c r="D144" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E144" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F144" s="6">
         <v>67</v>
       </c>
       <c r="G144" s="6">
-        <v>1347</v>
+        <v>1409</v>
       </c>
       <c r="H144" s="6">
         <v>5</v>
@@ -6736,16 +6736,16 @@
         <v>26</v>
       </c>
       <c r="D148" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E148" s="6">
         <v>1</v>
       </c>
       <c r="F148" s="6">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="G148" s="6">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="H148" s="6">
         <v>1</v>
@@ -6796,16 +6796,16 @@
         <v>26</v>
       </c>
       <c r="D150" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E150" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F150" s="6">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G150" s="6">
-        <v>227</v>
+        <v>317</v>
       </c>
       <c r="H150" s="6">
         <v>1</v>
@@ -6826,16 +6826,16 @@
         <v>26</v>
       </c>
       <c r="D151" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E151" s="6">
         <v>2</v>
       </c>
       <c r="F151" s="6">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G151" s="6">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="H151" s="6">
         <v>0</v>
@@ -6886,16 +6886,16 @@
         <v>26</v>
       </c>
       <c r="D153" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E153" s="6">
         <v>8</v>
       </c>
       <c r="F153" s="6">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G153" s="6">
-        <v>686</v>
+        <v>698</v>
       </c>
       <c r="H153" s="6">
         <v>1</v>
@@ -6916,16 +6916,16 @@
         <v>26</v>
       </c>
       <c r="D154" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E154" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F154" s="6">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G154" s="6">
-        <v>1232</v>
+        <v>1322</v>
       </c>
       <c r="H154" s="6">
         <v>0</v>
@@ -7006,16 +7006,16 @@
         <v>39</v>
       </c>
       <c r="D157" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E157" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F157" s="6">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G157" s="6">
-        <v>477</v>
+        <v>555</v>
       </c>
       <c r="H157" s="6">
         <v>2</v>
@@ -7036,16 +7036,16 @@
         <v>39</v>
       </c>
       <c r="D158" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E158" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F158" s="6">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G158" s="6">
-        <v>393</v>
+        <v>464</v>
       </c>
       <c r="H158" s="6">
         <v>1</v>
@@ -16816,16 +16816,16 @@
         <v>11</v>
       </c>
       <c r="D484" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E484" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F484" s="6">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G484" s="6">
-        <v>573</v>
+        <v>663</v>
       </c>
       <c r="H484" s="6">
         <v>0</v>
@@ -16876,22 +16876,22 @@
         <v>14</v>
       </c>
       <c r="D486" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E486" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F486" s="6">
         <v>81</v>
       </c>
       <c r="G486" s="6">
-        <v>1860</v>
+        <v>1950</v>
       </c>
       <c r="H486" s="6">
         <v>0</v>
       </c>
       <c r="I486" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J486" s="4"/>
     </row>
@@ -16936,16 +16936,16 @@
         <v>14</v>
       </c>
       <c r="D488" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E488" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F488" s="6">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G488" s="6">
-        <v>1485</v>
+        <v>1575</v>
       </c>
       <c r="H488" s="6">
         <v>0</v>
@@ -16966,16 +16966,16 @@
         <v>14</v>
       </c>
       <c r="D489" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E489" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F489" s="6">
         <v>80</v>
       </c>
       <c r="G489" s="6">
-        <v>1196</v>
+        <v>1286</v>
       </c>
       <c r="H489" s="6">
         <v>0</v>
@@ -17146,16 +17146,16 @@
         <v>14</v>
       </c>
       <c r="D495" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E495" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F495" s="6">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="G495" s="6">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="H495" s="6">
         <v>0</v>
@@ -17206,16 +17206,16 @@
         <v>26</v>
       </c>
       <c r="D497" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E497" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F497" s="6">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G497" s="6">
-        <v>1054</v>
+        <v>1071</v>
       </c>
       <c r="H497" s="6">
         <v>4</v>
@@ -17236,16 +17236,16 @@
         <v>26</v>
       </c>
       <c r="D498" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E498" s="6">
         <v>15</v>
       </c>
       <c r="F498" s="6">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G498" s="6">
-        <v>1202</v>
+        <v>1225</v>
       </c>
       <c r="H498" s="6">
         <v>0</v>
@@ -17296,22 +17296,22 @@
         <v>26</v>
       </c>
       <c r="D500" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E500" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F500" s="6">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G500" s="6">
-        <v>919</v>
+        <v>986</v>
       </c>
       <c r="H500" s="6">
+        <v>3</v>
+      </c>
+      <c r="I500" s="6">
         <v>2</v>
-      </c>
-      <c r="I500" s="6">
-        <v>1</v>
       </c>
       <c r="J500" s="4"/>
     </row>
@@ -17326,16 +17326,16 @@
         <v>26</v>
       </c>
       <c r="D501" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E501" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F501" s="6">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G501" s="6">
-        <v>1171</v>
+        <v>1261</v>
       </c>
       <c r="H501" s="6">
         <v>1</v>
@@ -17356,16 +17356,16 @@
         <v>26</v>
       </c>
       <c r="D502" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E502" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F502" s="6">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G502" s="6">
-        <v>996</v>
+        <v>1063</v>
       </c>
       <c r="H502" s="6">
         <v>1</v>
@@ -17386,19 +17386,19 @@
         <v>26</v>
       </c>
       <c r="D503" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E503" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F503" s="6">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G503" s="6">
-        <v>1886</v>
+        <v>1976</v>
       </c>
       <c r="H503" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I503" s="6">
         <v>1</v>
@@ -17476,16 +17476,16 @@
         <v>26</v>
       </c>
       <c r="D506" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E506" s="6">
         <v>6</v>
       </c>
       <c r="F506" s="6">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G506" s="6">
-        <v>460</v>
+        <v>483</v>
       </c>
       <c r="H506" s="6">
         <v>1</v>
@@ -17566,16 +17566,16 @@
         <v>39</v>
       </c>
       <c r="D509" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E509" s="6">
         <v>10</v>
       </c>
       <c r="F509" s="6">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G509" s="6">
-        <v>881</v>
+        <v>892</v>
       </c>
       <c r="H509" s="6">
         <v>4</v>
@@ -17596,16 +17596,16 @@
         <v>39</v>
       </c>
       <c r="D510" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E510" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F510" s="6">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G510" s="6">
-        <v>980</v>
+        <v>1059</v>
       </c>
       <c r="H510" s="6">
         <v>2</v>
@@ -17626,16 +17626,16 @@
         <v>39</v>
       </c>
       <c r="D511" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E511" s="6">
         <v>7</v>
       </c>
       <c r="F511" s="6">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G511" s="6">
-        <v>745</v>
+        <v>756</v>
       </c>
       <c r="H511" s="6">
         <v>3</v>
@@ -17656,7 +17656,7 @@
         <v>39</v>
       </c>
       <c r="D512" s="6">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E512" s="6">
         <v>13</v>
@@ -17665,7 +17665,7 @@
         <v>51</v>
       </c>
       <c r="G512" s="6">
-        <v>1317</v>
+        <v>1390</v>
       </c>
       <c r="H512" s="6">
         <v>3</v>
@@ -17686,16 +17686,16 @@
         <v>11</v>
       </c>
       <c r="D513" s="6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E513" s="6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F513" s="6">
         <v>90</v>
       </c>
       <c r="G513" s="6">
-        <v>2520</v>
+        <v>2610</v>
       </c>
       <c r="H513" s="6">
         <v>0</v>
@@ -17836,16 +17836,16 @@
         <v>14</v>
       </c>
       <c r="D518" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E518" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F518" s="6">
         <v>85</v>
       </c>
       <c r="G518" s="6">
-        <v>1869</v>
+        <v>1959</v>
       </c>
       <c r="H518" s="6">
         <v>0</v>
@@ -17866,16 +17866,16 @@
         <v>14</v>
       </c>
       <c r="D519" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E519" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F519" s="6">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G519" s="6">
-        <v>1144</v>
+        <v>1234</v>
       </c>
       <c r="H519" s="6">
         <v>0</v>
@@ -17896,16 +17896,16 @@
         <v>14</v>
       </c>
       <c r="D520" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E520" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F520" s="6">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G520" s="6">
-        <v>1347</v>
+        <v>1437</v>
       </c>
       <c r="H520" s="6">
         <v>0</v>
@@ -17956,16 +17956,16 @@
         <v>14</v>
       </c>
       <c r="D522" s="6">
+        <v>10</v>
+      </c>
+      <c r="E522" s="6">
         <v>9</v>
       </c>
-      <c r="E522" s="6">
-        <v>8</v>
-      </c>
       <c r="F522" s="6">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G522" s="6">
-        <v>675</v>
+        <v>765</v>
       </c>
       <c r="H522" s="6">
         <v>0</v>
@@ -18076,19 +18076,19 @@
         <v>26</v>
       </c>
       <c r="D526" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E526" s="6">
         <v>18</v>
       </c>
       <c r="F526" s="6">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G526" s="6">
-        <v>1613</v>
+        <v>1658</v>
       </c>
       <c r="H526" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I526" s="6">
         <v>2</v>
@@ -18106,16 +18106,16 @@
         <v>26</v>
       </c>
       <c r="D527" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E527" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F527" s="6">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G527" s="6">
-        <v>1167</v>
+        <v>1212</v>
       </c>
       <c r="H527" s="6">
         <v>0</v>
@@ -18136,16 +18136,16 @@
         <v>26</v>
       </c>
       <c r="D528" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E528" s="6">
         <v>2</v>
       </c>
       <c r="F528" s="6">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G528" s="6">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="H528" s="6">
         <v>1</v>
@@ -18166,16 +18166,16 @@
         <v>26</v>
       </c>
       <c r="D529" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E529" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F529" s="6">
         <v>72</v>
       </c>
       <c r="G529" s="6">
-        <v>1792</v>
+        <v>1867</v>
       </c>
       <c r="H529" s="6">
         <v>3</v>
@@ -18226,22 +18226,22 @@
         <v>26</v>
       </c>
       <c r="D531" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E531" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F531" s="6">
         <v>79</v>
       </c>
       <c r="G531" s="6">
-        <v>1887</v>
+        <v>1977</v>
       </c>
       <c r="H531" s="6">
         <v>1</v>
       </c>
       <c r="I531" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J531" s="4"/>
     </row>
@@ -18316,19 +18316,19 @@
         <v>26</v>
       </c>
       <c r="D534" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E534" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F534" s="6">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G534" s="6">
-        <v>1074</v>
+        <v>1159</v>
       </c>
       <c r="H534" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I534" s="6">
         <v>0</v>
@@ -18376,16 +18376,16 @@
         <v>26</v>
       </c>
       <c r="D536" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E536" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F536" s="6">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G536" s="6">
-        <v>458</v>
+        <v>537</v>
       </c>
       <c r="H536" s="6">
         <v>0</v>
@@ -18436,16 +18436,16 @@
         <v>39</v>
       </c>
       <c r="D538" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E538" s="6">
         <v>17</v>
       </c>
       <c r="F538" s="6">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G538" s="6">
-        <v>1265</v>
+        <v>1276</v>
       </c>
       <c r="H538" s="6">
         <v>2</v>
@@ -18496,22 +18496,22 @@
         <v>39</v>
       </c>
       <c r="D540" s="6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E540" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F540" s="6">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G540" s="6">
-        <v>953</v>
+        <v>1032</v>
       </c>
       <c r="H540" s="6">
         <v>5</v>
       </c>
       <c r="I540" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J540" s="4"/>
     </row>

</xml_diff>